<commit_message>
[PHOENIX-6396] -ui updated data file of lcms
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/legalCaseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/legalCaseTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="createLegalCaseData" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -46,13 +46,10 @@
     <t xml:space="preserve">testData1</t>
   </si>
   <si>
-    <t xml:space="preserve">High court</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contempt Case(CC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High court Hyderabad</t>
+    <t xml:space="preserve">District Court</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Original Suit(OS)</t>
   </si>
   <si>
     <t xml:space="preserve">Engineering</t>
@@ -71,7 +68,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -93,6 +90,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,8 +140,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -162,24 +169,24 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.9518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.1259259259259"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.7185185185185"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.4555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3814814814815"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.6148148148148"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.1074074074074"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -215,23 +222,23 @@
       <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>